<commit_message>
update palettes and start adding icons
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dev\TheGreatFlight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D490E3-F3C1-4F23-B8D7-645163FE3B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B7B5CA-A4E8-4637-A656-E7E8D453C193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6255" yWindow="2910" windowWidth="21600" windowHeight="12683" xr2:uid="{082D6853-836E-4E89-9CDF-2F28D2B9377F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{082D6853-836E-4E89-9CDF-2F28D2B9377F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="86">
   <si>
     <t>Top panel</t>
   </si>
@@ -267,6 +267,33 @@
   </si>
   <si>
     <t>MissileW</t>
+  </si>
+  <si>
+    <t>Build basic structure</t>
+  </si>
+  <si>
+    <t>Build advanced structure</t>
+  </si>
+  <si>
+    <t>Human Farm</t>
+  </si>
+  <si>
+    <t>Human Hall</t>
+  </si>
+  <si>
+    <t>Human Barracks</t>
+  </si>
+  <si>
+    <t>Human Mill</t>
+  </si>
+  <si>
+    <t>Human Smith</t>
+  </si>
+  <si>
+    <t>Human Church</t>
+  </si>
+  <si>
+    <t>Human Stable</t>
   </si>
 </sst>
 </file>
@@ -663,22 +690,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64E513D-2FA8-423D-AD0E-B874F4707F80}">
-  <dimension ref="A1:S73"/>
+  <dimension ref="A1:S82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.73046875" customWidth="1"/>
-    <col min="15" max="15" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -686,7 +713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P3" t="s">
         <v>69</v>
       </c>
@@ -694,7 +721,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>62</v>
       </c>
@@ -720,7 +747,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -748,7 +775,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -790,7 +817,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -817,7 +844,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -843,7 +870,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -874,7 +901,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -906,7 +933,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -940,7 +967,7 @@
         <v>6144</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -975,7 +1002,7 @@
         <v>6144</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1010,7 +1037,7 @@
         <v>13824</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1045,7 +1072,7 @@
         <v>13824</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1080,7 +1107,7 @@
         <v>5120</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1115,7 +1142,7 @@
         <v>13824</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1150,7 +1177,7 @@
         <v>9792</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1185,7 +1212,7 @@
         <v>6144</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1220,7 +1247,7 @@
         <v>6144</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1255,7 +1282,7 @@
         <v>6144</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1290,7 +1317,7 @@
         <v>6144</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1325,7 +1352,7 @@
         <v>14400</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1360,7 +1387,7 @@
         <v>14400</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1394,7 +1421,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -1428,7 +1455,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1462,7 +1489,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1496,7 +1523,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -1530,7 +1557,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1565,7 +1592,7 @@
         <v>14400</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1600,7 +1627,7 @@
         <v>14400</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1635,7 +1662,7 @@
         <v>9792</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="34" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1673,7 +1700,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1709,10 +1736,10 @@
       </c>
       <c r="P35">
         <f>(SUM(K5:K10)+K37+SUM(J13:J35)*2+Q4+Q5+Q6+Q7+S10)/1024</f>
-        <v>330.66015625</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
+        <v>336.56640625</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
@@ -1720,204 +1747,249 @@
         <v>3</v>
       </c>
       <c r="C37">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D37" t="s">
         <v>4</v>
       </c>
       <c r="E37">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G37" t="s">
         <v>57</v>
       </c>
       <c r="H37">
-        <f>COUNTA(A38:A80)</f>
-        <v>36</v>
+        <f>COUNTA(A38:A100)</f>
+        <v>45</v>
       </c>
       <c r="K37">
         <f>C37*E37*H37*B1/8</f>
-        <v>6912</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
+        <v>12960</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Spreadsheet to budget chipram
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dev\TheGreatFlight\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim Felgentreff\Documents\AmiWar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B7B5CA-A4E8-4637-A656-E7E8D453C193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DDBD5E-1851-4FBA-B1B1-DC5A70B51ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{082D6853-836E-4E89-9CDF-2F28D2B9377F}"/>
+    <workbookView xWindow="2340" yWindow="855" windowWidth="26340" windowHeight="14010" xr2:uid="{082D6853-836E-4E89-9CDF-2F28D2B9377F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="75">
   <si>
     <t>Top panel</t>
   </si>
@@ -261,39 +261,6 @@
   </si>
   <si>
     <t>17*2*2*3</t>
-  </si>
-  <si>
-    <t>Mouse action sprite</t>
-  </si>
-  <si>
-    <t>MissileW</t>
-  </si>
-  <si>
-    <t>Build basic structure</t>
-  </si>
-  <si>
-    <t>Build advanced structure</t>
-  </si>
-  <si>
-    <t>Human Farm</t>
-  </si>
-  <si>
-    <t>Human Hall</t>
-  </si>
-  <si>
-    <t>Human Barracks</t>
-  </si>
-  <si>
-    <t>Human Mill</t>
-  </si>
-  <si>
-    <t>Human Smith</t>
-  </si>
-  <si>
-    <t>Human Church</t>
-  </si>
-  <si>
-    <t>Human Stable</t>
   </si>
 </sst>
 </file>
@@ -690,13 +657,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64E513D-2FA8-423D-AD0E-B874F4707F80}">
-  <dimension ref="A1:S82"/>
+  <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="J65" sqref="J65"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
@@ -834,15 +801,6 @@
         <f>B7*C7*D7*B1/8</f>
         <v>11200</v>
       </c>
-      <c r="O7" t="s">
-        <v>75</v>
-      </c>
-      <c r="P7" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q7">
-        <v>68</v>
-      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -929,9 +887,6 @@
       <c r="K12" t="s">
         <v>72</v>
       </c>
-      <c r="O12" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -944,7 +899,7 @@
         <v>16</v>
       </c>
       <c r="D13" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -960,11 +915,11 @@
       </c>
       <c r="J13">
         <f>B13*C13*(D13*(E13+F13+G13)+H13)*B1/8</f>
-        <v>3072</v>
+        <v>6144</v>
       </c>
       <c r="K13">
         <f>J13*2</f>
-        <v>6144</v>
+        <v>12288</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -979,7 +934,7 @@
       </c>
       <c r="D14">
         <f>D13</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -995,11 +950,11 @@
       </c>
       <c r="J14">
         <f>B14*C14*(D14*(E14+F14+G14)+H14)*B1/8</f>
-        <v>3072</v>
+        <v>6144</v>
       </c>
       <c r="K14">
         <f t="shared" ref="K14:K35" si="0">J14*2</f>
-        <v>6144</v>
+        <v>12288</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1014,7 +969,7 @@
       </c>
       <c r="D15">
         <f t="shared" ref="D15:D25" si="1">D14</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1030,11 +985,11 @@
       </c>
       <c r="J15">
         <f>B15*C15*(D15*(E15+F15+G15+H15))*B1/8</f>
-        <v>6912</v>
+        <v>13824</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>13824</v>
+        <v>27648</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1049,7 +1004,7 @@
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1065,11 +1020,11 @@
       </c>
       <c r="J16">
         <f>B16*C16*(D16*(E16+F16+G16)+H16)*B1/8</f>
-        <v>6912</v>
+        <v>13824</v>
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>13824</v>
+        <v>27648</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1084,7 +1039,7 @@
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1100,11 +1055,11 @@
       </c>
       <c r="J17">
         <f>B17*C17*(D17*(E17+F17+G17)+H17)*B1/8</f>
-        <v>2560</v>
+        <v>5120</v>
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>5120</v>
+        <v>10240</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1119,7 +1074,7 @@
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1135,11 +1090,11 @@
       </c>
       <c r="J18">
         <f>B18*C18*(D18*(E18+F18+G18)+H18)*B1/8</f>
-        <v>6912</v>
+        <v>13824</v>
       </c>
       <c r="K18">
         <f t="shared" si="0"/>
-        <v>13824</v>
+        <v>27648</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1154,7 +1109,7 @@
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1170,11 +1125,11 @@
       </c>
       <c r="J19">
         <f>B19*C19*(D19*(E19+F19+G19)+H19)*B1/8</f>
-        <v>4896</v>
+        <v>9504</v>
       </c>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>9792</v>
+        <v>19008</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1189,7 +1144,7 @@
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1205,11 +1160,11 @@
       </c>
       <c r="J20">
         <f>B20*C20*(D20*(E20+F20+G20)+H20)*B1/8</f>
-        <v>3072</v>
+        <v>6144</v>
       </c>
       <c r="K20">
         <f t="shared" si="0"/>
-        <v>6144</v>
+        <v>12288</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1224,7 +1179,7 @@
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1240,11 +1195,11 @@
       </c>
       <c r="J21">
         <f>B21*C21*(D21*(E21+F21+G21)+H21)*B1/8</f>
-        <v>3072</v>
+        <v>6144</v>
       </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>6144</v>
+        <v>12288</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1259,7 +1214,7 @@
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1275,11 +1230,11 @@
       </c>
       <c r="J22">
         <f>B22*C22*(D22*(E22+F22+G22)+H22)*B1/8</f>
-        <v>3072</v>
+        <v>6144</v>
       </c>
       <c r="K22">
         <f t="shared" si="0"/>
-        <v>6144</v>
+        <v>12288</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1294,7 +1249,7 @@
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1310,11 +1265,11 @@
       </c>
       <c r="J23">
         <f>B23*C23*(D23*(E23+F23+G23)+H23)*B1/8</f>
-        <v>3072</v>
+        <v>6144</v>
       </c>
       <c r="K23">
         <f t="shared" si="0"/>
-        <v>6144</v>
+        <v>12288</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1329,7 +1284,7 @@
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1345,11 +1300,11 @@
       </c>
       <c r="J24">
         <f>B24*C24*(D24*(E24+F24+G24)+H24)*B1/8</f>
-        <v>7200</v>
+        <v>14112</v>
       </c>
       <c r="K24">
         <f t="shared" si="0"/>
-        <v>14400</v>
+        <v>28224</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1364,7 +1319,7 @@
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1380,11 +1335,11 @@
       </c>
       <c r="J25">
         <f>B25*C25*(D25*(E25+F25+G25)+H25)*B1/8</f>
-        <v>7200</v>
+        <v>14112</v>
       </c>
       <c r="K25">
         <f t="shared" si="0"/>
-        <v>14400</v>
+        <v>28224</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1569,7 +1524,7 @@
       </c>
       <c r="D31">
         <f>D13</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1585,11 +1540,11 @@
       </c>
       <c r="J31">
         <f>B31*C31*(D31*(E31+F31+G31)+H31)*B1/8</f>
-        <v>7200</v>
+        <v>14112</v>
       </c>
       <c r="K31">
         <f t="shared" si="0"/>
-        <v>14400</v>
+        <v>28224</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1604,7 +1559,7 @@
       </c>
       <c r="D32">
         <f t="shared" ref="D32:D35" si="2">D14</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1620,11 +1575,11 @@
       </c>
       <c r="J32">
         <f>B32*C32*(D32*(E32+F32+G32)+H32)*B1/8</f>
-        <v>7200</v>
+        <v>14112</v>
       </c>
       <c r="K32">
         <f t="shared" si="0"/>
-        <v>14400</v>
+        <v>28224</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -1639,7 +1594,7 @@
       </c>
       <c r="D33">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -1655,11 +1610,11 @@
       </c>
       <c r="J33">
         <f>B33*C33*(D33*(E33+F33+G33)+H33)*B1/8</f>
-        <v>4896</v>
+        <v>9504</v>
       </c>
       <c r="K33">
         <f t="shared" si="0"/>
-        <v>9792</v>
+        <v>19008</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1674,7 +1629,7 @@
       </c>
       <c r="D34">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -1690,11 +1645,11 @@
       </c>
       <c r="J34">
         <f>B34*C34*(D34*(E34+F34+G34)+H34)*B1/8</f>
-        <v>7200</v>
+        <v>14112</v>
       </c>
       <c r="K34">
         <f t="shared" si="0"/>
-        <v>14400</v>
+        <v>28224</v>
       </c>
       <c r="P34" s="3" t="s">
         <v>63</v>
@@ -1705,14 +1660,14 @@
         <v>38</v>
       </c>
       <c r="B35">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C35">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D35">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1728,15 +1683,15 @@
       </c>
       <c r="J35">
         <f>B35*C35*(D35*(E35+F35+G35)+H35)*B1/8</f>
-        <v>3072</v>
+        <v>13824</v>
       </c>
       <c r="K35">
         <f t="shared" si="0"/>
-        <v>6144</v>
+        <v>27648</v>
       </c>
       <c r="P35">
-        <f>(SUM(K5:K10)+K37+SUM(J13:J35)*2+Q4+Q5+Q6+Q7+S10)/1024</f>
-        <v>336.56640625</v>
+        <f>(SUM(K5:K187)+Q4+Q5+Q6+S10)/1024</f>
+        <v>518.59375</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -1747,24 +1702,24 @@
         <v>3</v>
       </c>
       <c r="C37">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D37" t="s">
         <v>4</v>
       </c>
       <c r="E37">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G37" t="s">
         <v>57</v>
       </c>
       <c r="H37">
-        <f>COUNTA(A38:A100)</f>
-        <v>45</v>
+        <f>COUNTA(A38:A80)</f>
+        <v>36</v>
       </c>
       <c r="K37">
         <f>C37*E37*H37*B1/8</f>
-        <v>12960</v>
+        <v>6912</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -1945,51 +1900,6 @@
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
begin changing color palette
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim Felgentreff\Documents\AmiWar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\greatflight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DDBD5E-1851-4FBA-B1B1-DC5A70B51ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7E4C64-16EB-4B86-BB7E-2348513AEA38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="855" windowWidth="26340" windowHeight="14010" xr2:uid="{082D6853-836E-4E89-9CDF-2F28D2B9377F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{082D6853-836E-4E89-9CDF-2F28D2B9377F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="76">
   <si>
     <t>Top panel</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>17*2*2*3</t>
+  </si>
+  <si>
+    <t>Pristine map</t>
   </si>
 </sst>
 </file>
@@ -361,9 +364,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -401,7 +404,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -507,7 +510,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -649,7 +652,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -659,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64E513D-2FA8-423D-AD0E-B874F4707F80}">
   <dimension ref="A1:S73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,18 +763,18 @@
       </c>
       <c r="G6">
         <f>ROUNDUP((B6+(B10/2))/B10, 0)</f>
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
         <v>61</v>
       </c>
       <c r="I6">
         <f>ROUNDUP((C6+(C10/2))/C10, 0)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="K6">
         <f>G6*I6*B10*C10*D6*B1/8</f>
-        <v>61440</v>
+        <v>53504</v>
       </c>
       <c r="O6" t="s">
         <v>66</v>
@@ -802,6 +805,26 @@
         <v>11200</v>
       </c>
     </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8">
+        <f>64*16</f>
+        <v>1024</v>
+      </c>
+      <c r="C8">
+        <f>64*16</f>
+        <v>1024</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f>B8*C8*D8*4/8</f>
+        <v>524288</v>
+      </c>
+    </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
@@ -833,17 +856,17 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C10">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>128</v>
       </c>
       <c r="K10">
         <f>B10*C10*D10*B1/8</f>
-        <v>65536</v>
+        <v>16384</v>
       </c>
       <c r="P10">
         <v>128</v>
@@ -1691,7 +1714,7 @@
       </c>
       <c r="P35">
         <f>(SUM(K5:K187)+Q4+Q5+Q6+S10)/1024</f>
-        <v>518.59375</v>
+        <v>974.84375</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -1905,5 +1928,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Calibri"&amp;10&amp;K000000 Confidential - Oracle Restricted&amp;1#_x000D_</oddHeader>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Confidential - Oracle Restricted</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>